<commit_message>
commit to revert -_-
</commit_message>
<xml_diff>
--- a/data/output/Section3_Logical.xlsx
+++ b/data/output/Section3_Logical.xlsx
@@ -738,7 +738,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -5271,7 +5271,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -5320,7 +5320,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -7052,7 +7052,7 @@
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K130" t="inlineStr">
@@ -7101,7 +7101,7 @@
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K131" t="inlineStr">
@@ -11944,7 +11944,7 @@
       </c>
       <c r="J226" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
@@ -11993,7 +11993,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -19029,7 +19029,7 @@
       </c>
       <c r="J365" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K365" t="inlineStr">
@@ -22291,7 +22291,7 @@
       </c>
       <c r="J429" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K429" t="inlineStr">
@@ -57122,7 +57122,7 @@
       </c>
       <c r="J1112" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K1112" t="inlineStr">
@@ -57477,7 +57477,7 @@
       </c>
       <c r="J1119" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K1119" t="inlineStr">
@@ -57526,7 +57526,7 @@
       </c>
       <c r="J1120" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K1120" t="inlineStr">
@@ -74456,7 +74456,7 @@
       </c>
       <c r="J1452" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K1452" t="inlineStr">
@@ -74760,7 +74760,7 @@
       </c>
       <c r="J1458" t="inlineStr">
         <is>
-          <t>Mild</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K1458" t="inlineStr">

</xml_diff>